<commit_message>
load owl-vit model when using time
</commit_message>
<xml_diff>
--- a/output/excel/single_120QAN07H-3 (UX8407_906QA416H)_20250729.xlsx
+++ b/output/excel/single_120QAN07H-3 (UX8407_906QA416H)_20250729.xlsx
@@ -484,12 +484,14 @@
           <t>典型/正常電池容量,Wh</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>無</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Page 1 (loc: cropped_image:Battery Label Artwork): "Rating:+15.6V==49.5Wh (Rated)"</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -532,7 +534,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Page 1 (loc: cropped_image:Battery Label Artwork): "Rating:+15.6V==49.5Wh"</t>
+          <t>Page 1 (loc: cropped_image:Battery Label Artwork): "Rating:+15.6V==49.5Wh (Rated)"</t>
         </is>
       </c>
     </row>
@@ -544,7 +546,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>主要語言為英文，並含部分中文、日文、德文等多語警告文字。檔案為電池標籤展開圖，頁碼固定為1。typical battery capacity (Wh) 未在標籤中明確提供，故為 null。</t>
+          <t>主要語言為英文，並含部分中文、日文、德文等多語警告文字。頁碼採絕對 1-based。此為電池標籤展開圖，所有數值均直接取自標籤印刷內容。</t>
         </is>
       </c>
     </row>

</xml_diff>